<commit_message>
added modified templates, changed import and export of solution with missions. Added import of missions data in template, modified deployment.
</commit_message>
<xml_diff>
--- a/data/template/Test3/template_in.xlsx
+++ b/data/template/Test3/template_in.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchtsp\Documents\projects\optima\data\template\Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636B5F75-51EE-454B-8BA1-2BB0784D3E59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC614B9-4FDD-4B98-AEE2-8837DD46DD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="maintenances" sheetId="1" r:id="rId1"/>
-    <sheet name="etats_initiaux" sheetId="2" r:id="rId2"/>
-    <sheet name="params" sheetId="3" r:id="rId3"/>
-    <sheet name="avions" sheetId="4" r:id="rId4"/>
-    <sheet name="exemple_maints" sheetId="5" r:id="rId5"/>
+    <sheet name="missions" sheetId="6" r:id="rId2"/>
+    <sheet name="etats_initiaux" sheetId="2" r:id="rId3"/>
+    <sheet name="params" sheetId="3" r:id="rId4"/>
+    <sheet name="avions" sheetId="4" r:id="rId5"/>
+    <sheet name="exemple_maints" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="131">
   <si>
     <t>maint</t>
   </si>
@@ -396,6 +398,48 @@
   </si>
   <si>
     <t>2019-06</t>
+  </si>
+  <si>
+    <t>mission</t>
+  </si>
+  <si>
+    <t>date_debut</t>
+  </si>
+  <si>
+    <t>date_fin</t>
+  </si>
+  <si>
+    <t>type_avion</t>
+  </si>
+  <si>
+    <t>nb_avions</t>
+  </si>
+  <si>
+    <t>nb_heures</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>2021-11</t>
+  </si>
+  <si>
+    <t>2022-04</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>2021-04</t>
+  </si>
+  <si>
+    <t>2019-07</t>
+  </si>
+  <si>
+    <t>2022-02</t>
   </si>
 </sst>
 </file>
@@ -533,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -558,6 +602,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -902,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16:D19"/>
     </sheetView>
   </sheetViews>
@@ -1064,6 +1109,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A4D43D-058C-4C58-B74C-F27941989F63}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
@@ -2567,7 +2711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2635,12 +2779,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,252 +2792,345 @@
     <col min="1" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="7">
         <v>2617</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="7">
         <v>2512</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B4" s="7">
         <v>2691</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="7">
         <v>2763</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B6" s="7">
         <v>1960</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>97</v>
       </c>
       <c r="B7" s="7">
         <v>4174</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="7">
         <v>5329</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B9" s="7">
         <v>2552</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="7">
         <v>2711</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B11" s="7">
         <v>2403</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>88</v>
       </c>
       <c r="B12" s="7">
         <v>1876</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="7">
         <v>2766</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="7">
         <v>4238</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="7">
         <v>2790</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="7">
         <v>2005</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="7">
         <v>4577</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B18" s="7">
         <v>2489</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="7">
         <v>2763</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B20" s="7">
         <v>2772</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="7">
         <v>2961</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B22" s="7">
         <v>4316</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>107</v>
       </c>
       <c r="B23" s="7">
         <v>4450</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>108</v>
       </c>
       <c r="B24" s="7">
         <v>3724</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B25" s="7">
         <v>2531</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>110</v>
       </c>
       <c r="B26" s="7">
         <v>4087</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B27" s="7">
         <v>2559</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>113</v>
       </c>
       <c r="B28" s="7">
         <v>2515</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>114</v>
       </c>
       <c r="B29" s="7">
         <v>2533</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B30" s="7">
         <v>5141</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B31" s="7">
         <v>2366</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2902,7 +3139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -3104,19 +3341,19 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="288.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Edited Dassault template and corrected some errors in the model.
</commit_message>
<xml_diff>
--- a/data/template/Test3/template_in.xlsx
+++ b/data/template/Test3/template_in.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchtsp\Documents\projects\optima\data\template\Test3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC614B9-4FDD-4B98-AEE2-8837DD46DD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055CAA51-DD37-46A3-9455-61DBBA68F949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="634" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="maintenances" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="132">
   <si>
     <t>maint</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>2022-02</t>
+  </si>
+  <si>
+    <t>2020-04</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1116,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1149,7 @@
         <v>129</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1195,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>